<commit_message>
cleaning and organizing revelle ml means
</commit_message>
<xml_diff>
--- a/data/ctd-cnv/RR1804/P2_2018/deep_chl/Station32_integrated_DCM_matlab.xlsx
+++ b/data/ctd-cnv/RR1804/P2_2018/deep_chl/Station32_integrated_DCM_matlab.xlsx
@@ -13,19 +13,22 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Cast</t>
   </si>
   <si>
     <t xml:space="preserve">StartTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartTime matlab datenum</t>
   </si>
   <si>
     <t xml:space="preserve">Int chl fluor</t>
@@ -143,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -154,7 +157,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="19.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,6 +176,9 @@
       <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -182,15 +188,16 @@
         <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="0" t="n">
         <v>15.92853</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>177.7587</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>45.691</v>
       </c>
     </row>
@@ -204,13 +211,14 @@
       <c r="C3" s="2" t="n">
         <v>43205.6291898148</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2"/>
+      <c r="E3" s="0" t="n">
         <v>15.70438</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>173.0129</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>47.779</v>
       </c>
     </row>
@@ -224,13 +232,14 @@
       <c r="C4" s="2" t="n">
         <v>43205.9178587963</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2"/>
+      <c r="E4" s="0" t="n">
         <v>14.91336</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>172.9927</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>51.398</v>
       </c>
     </row>
@@ -244,13 +253,14 @@
       <c r="C5" s="2" t="n">
         <v>43206.6271064815</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2"/>
+      <c r="E5" s="0" t="n">
         <v>14.53045</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>177.625</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>46.232</v>
       </c>
     </row>
@@ -264,13 +274,14 @@
       <c r="C6" s="2" t="n">
         <v>43207.6272685185</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2"/>
+      <c r="E6" s="0" t="n">
         <v>11.04443</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <v>150.4668</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>43.161</v>
       </c>
     </row>
@@ -284,13 +295,14 @@
       <c r="C7" s="2" t="n">
         <v>43207.8778703704</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2"/>
+      <c r="E7" s="0" t="n">
         <v>11.9219</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>155.0208</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>49.977</v>
       </c>
     </row>
@@ -304,13 +316,14 @@
       <c r="C8" s="2" t="n">
         <v>43208.6271180556</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2"/>
+      <c r="E8" s="0" t="n">
         <v>12.29344</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>187.0308</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>65.163</v>
       </c>
     </row>
@@ -324,13 +337,14 @@
       <c r="C9" s="2" t="n">
         <v>43208.9204282407</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2"/>
+      <c r="E9" s="0" t="n">
         <v>10.97383</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>136.6731</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>47.955</v>
       </c>
     </row>
@@ -344,13 +358,14 @@
       <c r="C10" s="2" t="n">
         <v>43209.0944097222</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2"/>
+      <c r="E10" s="0" t="n">
         <v>10.39415</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="F10" s="0" t="n">
         <v>136.7008</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>46.091</v>
       </c>
     </row>
@@ -364,14 +379,19 @@
       <c r="C11" s="2" t="n">
         <v>43209.2550347222</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2"/>
+      <c r="E11" s="0" t="n">
         <v>17.16247</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <v>177.6435</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="G11" s="0" t="n">
         <v>53.381</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">G11-$G$11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,14 +404,19 @@
       <c r="C12" s="2" t="n">
         <v>43209.5044675926</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2"/>
+      <c r="E12" s="0" t="n">
         <v>13.34241</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="F12" s="0" t="n">
         <v>154.912</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>50.191</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">G12-$G$11</f>
+        <v>-3.19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,14 +429,19 @@
       <c r="C13" s="2" t="n">
         <v>43209.5950578704</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2"/>
+      <c r="E13" s="0" t="n">
         <v>10.43863</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>127.4998</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>40.507</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">G13-$G$11</f>
+        <v>-12.874</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,14 +454,19 @@
       <c r="C14" s="2" t="n">
         <v>43209.7540393518</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2"/>
+      <c r="E14" s="0" t="n">
         <v>12.44628</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="F14" s="0" t="n">
         <v>163.9449</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="G14" s="0" t="n">
         <v>51.238</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">G14-$G$11</f>
+        <v>-2.143</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,14 +479,19 @@
       <c r="C15" s="2" t="n">
         <v>43209.9997453704</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2"/>
+      <c r="E15" s="0" t="n">
         <v>12.57341</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="F15" s="0" t="n">
         <v>200.376</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="G15" s="0" t="n">
         <v>69.93</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">G15-$G$11</f>
+        <v>16.549</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,14 +504,19 @@
       <c r="C16" s="2" t="n">
         <v>43210.2547222222</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2"/>
+      <c r="E16" s="0" t="n">
         <v>12.30568</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="F16" s="0" t="n">
         <v>154.7222</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="G16" s="0" t="n">
         <v>58.535</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">G16-$G$11</f>
+        <v>5.154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,14 +529,19 @@
       <c r="C17" s="2" t="n">
         <v>43210.4596759259</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2"/>
+      <c r="E17" s="0" t="n">
         <v>21.0681</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="F17" s="0" t="n">
         <v>232.1141</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="G17" s="0" t="n">
         <v>77.788</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">G17-$G$11</f>
+        <v>24.407</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,23 +554,28 @@
       <c r="C18" s="2" t="n">
         <v>43210.940474537</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2"/>
+      <c r="E18" s="0" t="n">
         <v>10.88932</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="F18" s="0" t="n">
         <v>154.7883</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="G18" s="0" t="n">
         <v>54.208</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">G18-$G$11</f>
+        <v>0.826999999999998</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>